<commit_message>
Prueba a cuentas bancarias 0.1
</commit_message>
<xml_diff>
--- a/MercuryTours/Resources/datapool/usuarios.xlsx
+++ b/MercuryTours/Resources/datapool/usuarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12900" windowHeight="3390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13965" windowHeight="2820"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Andres Henao</t>
   </si>
@@ -114,16 +114,36 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>lzapata@edeq.com</t>
+  </si>
+  <si>
+    <t>mgarcia@edeq.com</t>
+  </si>
+  <si>
+    <t>dflores@edeq.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,10 +166,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -158,8 +179,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,14 +491,15 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -596,6 +623,20 @@
         <v>15</v>
       </c>
     </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
     </row>
@@ -606,7 +647,12 @@
       <c r="C9" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="C6" r:id="rId2"/>
+    <hyperlink ref="D6" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>